<commit_message>
Change contents branch label to _contents. Rename xlsx files to match their form_id (so conversion script can run).
</commit_message>
<xml_diff>
--- a/form-files/tables/complex_validate_test/forms/complex_validate_test/complex_validate_test.xlsx
+++ b/form-files/tables/complex_validate_test/forms/complex_validate_test/complex_validate_test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="18740" windowHeight="10560"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="18740" windowHeight="10560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>comments</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>user_info finalize</t>
-  </si>
-  <si>
-    <t>contents</t>
   </si>
 </sst>
 </file>
@@ -713,23 +710,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="15" width="18.33203125" customWidth="1"/>
-    <col min="16" max="16" width="24.1640625" customWidth="1"/>
-    <col min="17" max="18" width="18.33203125" customWidth="1"/>
+    <col min="1" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="7" width="18.36328125" customWidth="1"/>
+    <col min="8" max="8" width="28.6328125" customWidth="1"/>
+    <col min="9" max="15" width="18.36328125" customWidth="1"/>
+    <col min="16" max="16" width="24.1796875" customWidth="1"/>
+    <col min="17" max="18" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,13 +782,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="17.5" customHeight="1">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>36</v>
       </c>
@@ -805,17 +802,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>44</v>
       </c>
@@ -826,12 +823,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
         <v>44</v>
       </c>
@@ -842,17 +839,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
         <v>44</v>
       </c>
@@ -863,17 +860,17 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>44</v>
       </c>
@@ -884,17 +881,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
         <v>44</v>
       </c>
@@ -905,29 +902,19 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="C22" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -948,22 +935,22 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="1" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="33.6328125" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" customWidth="1"/>
-    <col min="15" max="15" width="30.1640625" customWidth="1"/>
-    <col min="16" max="16" width="33.6640625" customWidth="1"/>
-    <col min="17" max="18" width="13.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.5" customWidth="1"/>
+    <col min="12" max="13" width="13.6328125" customWidth="1"/>
+    <col min="14" max="14" width="20.36328125" customWidth="1"/>
+    <col min="15" max="15" width="30.1796875" customWidth="1"/>
+    <col min="16" max="16" width="33.6328125" customWidth="1"/>
+    <col min="17" max="18" width="13.6328125" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>44</v>
       </c>
@@ -1033,7 +1020,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>61</v>
       </c>
@@ -1062,7 +1049,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
         <v>52</v>
       </c>
@@ -1091,7 +1078,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>61</v>
       </c>
@@ -1138,18 +1125,18 @@
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" customWidth="1"/>
-    <col min="15" max="16" width="34.6640625" customWidth="1"/>
-    <col min="17" max="18" width="15.33203125" customWidth="1"/>
-    <col min="19" max="19" width="16.5" customWidth="1"/>
+    <col min="1" max="7" width="15.36328125" customWidth="1"/>
+    <col min="8" max="8" width="27.1796875" customWidth="1"/>
+    <col min="9" max="13" width="15.36328125" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" customWidth="1"/>
+    <col min="15" max="16" width="34.6328125" customWidth="1"/>
+    <col min="17" max="18" width="15.36328125" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1195,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>44</v>
       </c>
@@ -1219,7 +1206,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>96</v>
       </c>
@@ -1257,12 +1244,12 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1276,7 +1263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1290,7 +1277,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1304,7 +1291,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1332,20 +1319,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="7" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" customWidth="1"/>
+    <col min="5" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -1365,7 +1352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1377,7 +1364,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1389,7 +1376,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17" customHeight="1">
+    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>79</v>
       </c>
@@ -1403,7 +1390,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
@@ -1417,7 +1404,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1431,7 +1418,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1445,7 +1432,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Change 'assign' to use 'calculation' as the column name for the formula to assign to the name. Remove 'default' from prompts. Can specify an value default on the model element, or use 'assign'.
</commit_message>
<xml_diff>
--- a/form-files/tables/complex_validate_test/forms/complex_validate_test/complex_validate_test.xlsx
+++ b/form-files/tables/complex_validate_test/forms/complex_validate_test/complex_validate_test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="2320" windowWidth="28400" windowHeight="15060"/>
+    <workbookView xWindow="5900" yWindow="2320" windowWidth="25820" windowHeight="15060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="103">
   <si>
     <t>comments</t>
   </si>
@@ -713,24 +713,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
-    <col min="9" max="15" width="18.33203125" customWidth="1"/>
-    <col min="16" max="16" width="24.1640625" customWidth="1"/>
-    <col min="17" max="18" width="18.33203125" customWidth="1"/>
-    <col min="19" max="19" width="25.83203125" customWidth="1"/>
+    <col min="1" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="7" width="18.36328125" customWidth="1"/>
+    <col min="8" max="8" width="28.6328125" customWidth="1"/>
+    <col min="9" max="15" width="18.36328125" customWidth="1"/>
+    <col min="16" max="16" width="24.1796875" customWidth="1"/>
+    <col min="17" max="17" width="18.36328125" customWidth="1"/>
+    <col min="18" max="18" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,19 +783,16 @@
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="7" customFormat="1" ht="17.5" customHeight="1">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>36</v>
       </c>
@@ -808,21 +805,21 @@
       <c r="I3" t="s">
         <v>64</v>
       </c>
-      <c r="S3" t="b">
+      <c r="R3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
         <v>44</v>
       </c>
@@ -832,16 +829,16 @@
       <c r="I6" t="s">
         <v>65</v>
       </c>
-      <c r="S6" t="b">
+      <c r="R6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
         <v>44</v>
       </c>
@@ -851,21 +848,21 @@
       <c r="I8" t="s">
         <v>66</v>
       </c>
-      <c r="S8" t="b">
+      <c r="R8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
         <v>44</v>
       </c>
@@ -875,21 +872,21 @@
       <c r="I11" t="s">
         <v>67</v>
       </c>
-      <c r="S11" t="b">
+      <c r="R11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>44</v>
       </c>
@@ -899,21 +896,21 @@
       <c r="I14" t="s">
         <v>68</v>
       </c>
-      <c r="S14" t="b">
+      <c r="R14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="3:19">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
         <v>44</v>
       </c>
@@ -923,21 +920,21 @@
       <c r="I17" t="s">
         <v>70</v>
       </c>
-      <c r="S17" t="b">
+      <c r="R17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:19">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="3:19">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="3:19">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>49</v>
       </c>
@@ -954,29 +951,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="1" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="33.6328125" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" customWidth="1"/>
-    <col min="15" max="15" width="30.1640625" customWidth="1"/>
-    <col min="16" max="16" width="33.6640625" customWidth="1"/>
-    <col min="17" max="18" width="13.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.5" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" customWidth="1"/>
+    <col min="12" max="13" width="13.6328125" customWidth="1"/>
+    <col min="14" max="14" width="20.36328125" customWidth="1"/>
+    <col min="15" max="15" width="30.1796875" customWidth="1"/>
+    <col min="16" max="16" width="33.6328125" customWidth="1"/>
+    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="18" max="18" width="16.453125" customWidth="1"/>
+    <col min="19" max="19" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,16 +1026,13 @@
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>44</v>
       </c>
@@ -1048,11 +1042,11 @@
       <c r="I2" t="s">
         <v>81</v>
       </c>
-      <c r="T2" t="b">
+      <c r="S2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>61</v>
       </c>
@@ -1077,11 +1071,11 @@
       <c r="P3" t="s">
         <v>76</v>
       </c>
-      <c r="S3" t="s">
+      <c r="R3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
         <v>52</v>
       </c>
@@ -1106,11 +1100,11 @@
       <c r="P4" t="s">
         <v>75</v>
       </c>
-      <c r="S4" t="s">
+      <c r="R4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>61</v>
       </c>
@@ -1135,7 +1129,7 @@
       <c r="P5" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s">
+      <c r="R5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1151,25 +1145,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" customWidth="1"/>
-    <col min="15" max="16" width="34.6640625" customWidth="1"/>
-    <col min="17" max="18" width="15.33203125" customWidth="1"/>
-    <col min="19" max="19" width="16.5" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" customWidth="1"/>
+    <col min="1" max="7" width="15.36328125" customWidth="1"/>
+    <col min="8" max="8" width="27.1796875" customWidth="1"/>
+    <col min="9" max="13" width="15.36328125" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" customWidth="1"/>
+    <col min="15" max="16" width="34.6328125" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" customWidth="1"/>
+    <col min="18" max="18" width="16.453125" customWidth="1"/>
+    <col min="19" max="19" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,16 +1216,13 @@
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>44</v>
       </c>
@@ -1241,11 +1232,11 @@
       <c r="I2" t="s">
         <v>59</v>
       </c>
-      <c r="T2" t="b">
+      <c r="S2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>96</v>
       </c>
@@ -1261,7 +1252,7 @@
       <c r="M3" t="b">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
+      <c r="R3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1283,12 +1274,12 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1302,7 +1293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1316,7 +1307,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1330,7 +1321,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1362,16 +1353,16 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="7" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" customWidth="1"/>
+    <col min="5" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -1391,7 +1382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1403,7 +1394,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1415,7 +1406,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17" customHeight="1">
+    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>79</v>
       </c>
@@ -1429,7 +1420,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
@@ -1443,7 +1434,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1457,7 +1448,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1471,7 +1462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>